<commit_message>
Updated on 20 Jan 2020
</commit_message>
<xml_diff>
--- a/STLP/Documents/STLP_Time_Log.xlsx
+++ b/STLP/Documents/STLP_Time_Log.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24D5BD7-9250-416C-9462-B29FA906A1ED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB72F61-8497-4863-9C8F-C448F772E37A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33090" yWindow="945" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="50">
   <si>
     <t>Date and Time Logging</t>
   </si>
@@ -226,14 +226,17 @@
     <t>3.30 hrs carried over from last week</t>
   </si>
   <si>
-    <t>0:30 hr carried over</t>
+    <t>01:00 hour carried over from last week</t>
+  </si>
+  <si>
+    <t>Pause till further notice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,12 +280,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -379,18 +376,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -419,9 +410,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,10 +434,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -726,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32:F36"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,7 +730,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" style="27" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" style="25" customWidth="1"/>
     <col min="18" max="18" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -816,11 +809,11 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -878,47 +871,47 @@
       <c r="N9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="22" t="s">
+      <c r="O9" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="28" t="s">
+      <c r="P9" s="40"/>
+      <c r="Q9" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="24" t="s">
+      <c r="R9" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="S9" s="24" t="s">
+      <c r="S9" s="23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30">
+    <row r="10" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28">
         <v>43801</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="33">
+      <c r="C10" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="31">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="31">
         <v>0.875</v>
       </c>
-      <c r="F10" s="33">
-        <f t="shared" ref="F10:F28" si="0">E10-D10</f>
+      <c r="F10" s="31">
+        <f t="shared" ref="F10:F16" si="0">E10-D10</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
       <c r="M10" s="19">
         <f>SUM(L10:L31)</f>
         <v>0</v>
@@ -927,13 +920,13 @@
         <f>F9-M10</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O10" s="39" t="s">
+      <c r="O10" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P10" s="39" t="s">
+      <c r="P10" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Q10" s="36"/>
+      <c r="Q10" s="34"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -1009,7 +1002,7 @@
       <c r="H13" t="s">
         <v>21</v>
       </c>
-      <c r="Q13" s="29">
+      <c r="Q13" s="27">
         <v>0.125</v>
       </c>
       <c r="R13" s="11"/>
@@ -1043,7 +1036,7 @@
       <c r="M14" s="11">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="Q14" s="29">
+      <c r="Q14" s="27">
         <v>0.125</v>
       </c>
       <c r="R14" s="11"/>
@@ -1083,7 +1076,7 @@
       <c r="P15" s="11">
         <v>0.47152777777777777</v>
       </c>
-      <c r="Q15" s="29">
+      <c r="Q15" s="27">
         <v>0.16319444444444445</v>
       </c>
       <c r="R15" s="11"/>
@@ -1121,7 +1114,7 @@
       <c r="P16" s="11">
         <v>0.97152777777777777</v>
       </c>
-      <c r="Q16" s="29">
+      <c r="Q16" s="27">
         <v>0.27361111111111108</v>
       </c>
       <c r="R16" s="11"/>
@@ -1157,7 +1150,7 @@
       <c r="P17" s="11">
         <v>0.90486111111111101</v>
       </c>
-      <c r="Q17" s="29">
+      <c r="Q17" s="27">
         <v>0.21388888888888891</v>
       </c>
       <c r="R17" s="11">
@@ -1167,42 +1160,42 @@
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+    <row r="18" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28">
         <v>43822</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="33">
+      <c r="C18" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="31">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="31">
         <v>0.625</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="31">
         <v>0.16666666666666666</v>
       </c>
-      <c r="G18" s="33">
+      <c r="G18" s="31">
         <v>0.16666666666666666</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="O18" s="33">
+      <c r="O18" s="31">
         <v>0.48819444444444443</v>
       </c>
-      <c r="P18" s="33">
+      <c r="P18" s="31">
         <v>0.95972222222222225</v>
       </c>
-      <c r="Q18" s="35">
+      <c r="Q18" s="33">
         <v>0.16527777777777777</v>
       </c>
-      <c r="R18" s="33"/>
-      <c r="S18" s="33"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
@@ -1235,7 +1228,7 @@
       <c r="P19" s="11">
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q19" s="29">
+      <c r="Q19" s="27">
         <v>0.21249999999999999</v>
       </c>
       <c r="R19" s="11"/>
@@ -1247,13 +1240,13 @@
       <c r="B20" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="38" t="s">
         <v>45</v>
       </c>
       <c r="H20" t="s">
         <v>37</v>
       </c>
-      <c r="Q20" s="29">
+      <c r="Q20" s="27">
         <v>0</v>
       </c>
       <c r="R20" s="11"/>
@@ -1289,7 +1282,7 @@
       <c r="P21" s="11">
         <v>0.86249999999999993</v>
       </c>
-      <c r="Q21" s="29">
+      <c r="Q21" s="27">
         <v>0.19999999999999998</v>
       </c>
       <c r="R21" s="11"/>
@@ -1325,7 +1318,7 @@
       <c r="P22" s="11">
         <v>0.98958333333333337</v>
       </c>
-      <c r="Q22" s="29">
+      <c r="Q22" s="27">
         <v>0.26458333333333334</v>
       </c>
       <c r="R22" s="11"/>
@@ -1349,7 +1342,7 @@
       <c r="F23" s="11">
         <v>0.15277777777777776</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="22" t="s">
         <v>40</v>
       </c>
       <c r="H23" t="s">
@@ -1361,7 +1354,7 @@
       <c r="P23" s="11">
         <v>0.8666666666666667</v>
       </c>
-      <c r="Q23" s="29">
+      <c r="Q23" s="27">
         <v>0.15277777777777776</v>
       </c>
       <c r="R23" s="11"/>
@@ -1385,7 +1378,7 @@
       <c r="F24" s="11">
         <v>0.18402777777777779</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="22" t="s">
         <v>40</v>
       </c>
       <c r="H24" t="s">
@@ -1397,40 +1390,40 @@
       <c r="P24" s="11">
         <v>0.98958333333333337</v>
       </c>
-      <c r="Q24" s="29">
+      <c r="Q24" s="27">
         <v>0.18402777777777779</v>
       </c>
-      <c r="R24" s="25" t="s">
+      <c r="R24" s="24" t="s">
         <v>44</v>
       </c>
       <c r="S24" s="11">
         <v>0.34722222222222227</v>
       </c>
     </row>
-    <row r="25" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30">
+    <row r="25" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28">
         <v>43829</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="33">
+      <c r="C25" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="31">
         <v>0.375</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="31">
         <v>0.33333333333333331</v>
       </c>
-      <c r="H25" s="34" t="s">
+      <c r="H25" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="O25" s="33"/>
-      <c r="Q25" s="36"/>
+      <c r="O25" s="31"/>
+      <c r="Q25" s="34"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
@@ -1457,7 +1450,7 @@
       <c r="P26" s="11">
         <v>0.8847222222222223</v>
       </c>
-      <c r="Q26" s="29">
+      <c r="Q26" s="27">
         <v>0.4826388888888889</v>
       </c>
     </row>
@@ -1486,7 +1479,7 @@
       <c r="P27" s="11">
         <v>6.458333333333334E-2</v>
       </c>
-      <c r="Q27" s="29">
+      <c r="Q27" s="27">
         <v>6.25E-2</v>
       </c>
     </row>
@@ -1515,7 +1508,7 @@
       <c r="P28" s="11">
         <v>0.83888888888888891</v>
       </c>
-      <c r="Q28" s="29">
+      <c r="Q28" s="27">
         <v>0.10208333333333335</v>
       </c>
     </row>
@@ -1544,7 +1537,7 @@
       <c r="P29" s="11">
         <v>0.84375</v>
       </c>
-      <c r="Q29" s="29">
+      <c r="Q29" s="27">
         <v>0.28125</v>
       </c>
     </row>
@@ -1564,7 +1557,7 @@
       <c r="E30" s="11">
         <v>0.86805555555555547</v>
       </c>
-      <c r="F30" s="42">
+      <c r="F30" s="39">
         <v>0.14583333333333334</v>
       </c>
       <c r="O30" s="11">
@@ -1573,7 +1566,7 @@
       <c r="P30" s="11">
         <v>0.87013888888888891</v>
       </c>
-      <c r="Q30" s="29">
+      <c r="Q30" s="27">
         <v>5.7638888888888885E-2</v>
       </c>
     </row>
@@ -1584,7 +1577,7 @@
       <c r="B31" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="38" t="s">
         <v>45</v>
       </c>
       <c r="R31" s="11">
@@ -1594,35 +1587,35 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="32" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30">
+    <row r="32" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="28">
         <v>43836</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="33">
+      <c r="C32" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E32" s="33">
+      <c r="E32" s="31">
         <v>0.875</v>
       </c>
-      <c r="F32" s="33">
+      <c r="F32" s="31">
         <v>0.16666666666666666</v>
       </c>
-      <c r="H32" s="34" t="s">
+      <c r="H32" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="O32" s="33">
+      <c r="O32" s="31">
         <v>0.83194444444444438</v>
       </c>
-      <c r="P32" s="33">
+      <c r="P32" s="31">
         <v>0.90694444444444444</v>
       </c>
-      <c r="Q32" s="35">
+      <c r="Q32" s="33">
         <v>0.1875</v>
       </c>
     </row>
@@ -1633,8 +1626,8 @@
       <c r="B33" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="21" t="s">
-        <v>23</v>
+      <c r="C33" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="D33" s="11">
         <v>0.52083333333333337</v>
@@ -1651,7 +1644,7 @@
       <c r="P33" s="11">
         <v>0.97152777777777777</v>
       </c>
-      <c r="Q33" s="29">
+      <c r="Q33" s="27">
         <v>0.18819444444444444</v>
       </c>
     </row>
@@ -1662,8 +1655,8 @@
       <c r="B34" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="21" t="s">
-        <v>23</v>
+      <c r="C34" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="D34" s="11">
         <v>0.6875</v>
@@ -1680,7 +1673,7 @@
       <c r="P34" s="11">
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="Q34" s="29">
+      <c r="Q34" s="27">
         <v>0.14930555555555555</v>
       </c>
     </row>
@@ -1691,8 +1684,8 @@
       <c r="B35" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="21" t="s">
-        <v>23</v>
+      <c r="C35" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="D35" s="11">
         <v>0.75</v>
@@ -1709,7 +1702,7 @@
       <c r="P35" s="11">
         <v>2.5694444444444447E-2</v>
       </c>
-      <c r="Q35" s="29">
+      <c r="Q35" s="27">
         <v>0.20347222222222219</v>
       </c>
     </row>
@@ -1720,8 +1713,8 @@
       <c r="B36" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="21" t="s">
-        <v>23</v>
+      <c r="C36" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="D36" s="11">
         <v>0.75</v>
@@ -1738,7 +1731,7 @@
       <c r="P36" s="11">
         <v>0.89930555555555547</v>
       </c>
-      <c r="Q36" s="29">
+      <c r="Q36" s="27">
         <v>0.12916666666666668</v>
       </c>
     </row>
@@ -1749,7 +1742,7 @@
       <c r="B37" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="40" t="s">
+      <c r="C37" s="38" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1760,14 +1753,241 @@
       <c r="B38" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" s="38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H39" t="s">
+    <row r="39" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="28">
+        <v>43843</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="31">
+        <v>0.78125</v>
+      </c>
+      <c r="E39" s="31">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="F39" s="31">
+        <f>E39-D39</f>
+        <v>0.19791666666666663</v>
+      </c>
+      <c r="H39" s="31" t="s">
         <v>48</v>
       </c>
+      <c r="O39" s="31">
+        <v>0.77986111111111101</v>
+      </c>
+      <c r="P39" s="31">
+        <v>0.98541666666666661</v>
+      </c>
+      <c r="Q39" s="33">
+        <v>0.20069444444444443</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>43844</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="11">
+        <v>0.78125</v>
+      </c>
+      <c r="E40" s="11">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="F40" s="42">
+        <f>E40-D40</f>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="O40" s="11">
+        <v>0.77847222222222223</v>
+      </c>
+      <c r="P40" s="11">
+        <v>0.99791666666666667</v>
+      </c>
+      <c r="Q40" s="27">
+        <v>0.18402777777777779</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>43845</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="11">
+        <v>0.71875</v>
+      </c>
+      <c r="E41" s="11">
+        <v>0.8125</v>
+      </c>
+      <c r="F41" s="42">
+        <f>E41-D41</f>
+        <v>9.375E-2</v>
+      </c>
+      <c r="O41" s="11">
+        <v>0.71388888888888891</v>
+      </c>
+      <c r="P41" s="11">
+        <v>0.98888888888888893</v>
+      </c>
+      <c r="Q41" s="27">
+        <v>9.5138888888888884E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>43846</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="11">
+        <v>0.71875</v>
+      </c>
+      <c r="E42" s="11">
+        <v>0.90625</v>
+      </c>
+      <c r="F42" s="42">
+        <f>E42-D42</f>
+        <v>0.1875</v>
+      </c>
+      <c r="O42" s="11">
+        <v>0.72013888888888899</v>
+      </c>
+      <c r="P42" s="11">
+        <v>0.9604166666666667</v>
+      </c>
+      <c r="Q42" s="27">
+        <v>0.19513888888888889</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>43847</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="11">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="E43" s="11">
+        <v>0.84375</v>
+      </c>
+      <c r="F43" s="42">
+        <f>E43-D43</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="O43" s="11">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="P43" s="11">
+        <v>0.8618055555555556</v>
+      </c>
+      <c r="Q43" s="27">
+        <v>4.6527777777777779E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
+        <v>43848</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="11">
+        <v>0.8125</v>
+      </c>
+      <c r="E44" s="11">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F44" s="42">
+        <f>E44-D44</f>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="O44" s="11">
+        <v>0.80694444444444446</v>
+      </c>
+      <c r="P44" s="11">
+        <v>0.93611111111111101</v>
+      </c>
+      <c r="Q44" s="27">
+        <v>0.12708333333333333</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="9">
+        <v>43849</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="E45" s="11">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F45" s="42">
+        <f>E45-D45</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="O45" s="11">
+        <v>2.5694444444444447E-2</v>
+      </c>
+      <c r="P45" s="11">
+        <v>0.81666666666666676</v>
+      </c>
+      <c r="Q45" s="27">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
+        <v>43850</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>